<commit_message>
Integrated the macro & epidemiological models
Allow for different time steps.
</commit_message>
<xml_diff>
--- a/io/us_io_2019.xlsx
+++ b/io/us_io_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\epidemic-macro-model\io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DDB988-B786-4E89-BA6D-D5FF29EABB20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABCA14E-46E1-4D95-9971-E29C346EFC0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IO matrix (proc)" sheetId="6" r:id="rId1"/>
@@ -1183,11 +1183,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59779103-7F10-45DB-8408-304EC7FA3E3C}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2691,7 +2691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
@@ -4428,8 +4428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F43" activeCellId="1" sqref="C43 F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7309,8 +7309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>